<commit_message>
Cambios en los términos de búsquedas de referencias en la app.
</commit_message>
<xml_diff>
--- a/codigoFuente/SLR/templates/template.xlsx
+++ b/codigoFuente/SLR/templates/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="9555" windowHeight="7740" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="9555" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Study results</t>
   </si>
@@ -50,12 +50,6 @@
     <t>Source</t>
   </si>
   <si>
-    <t>Search Terms</t>
-  </si>
-  <si>
-    <t>Search Scope</t>
-  </si>
-  <si>
     <t>Results</t>
   </si>
   <si>
@@ -105,6 +99,9 @@
   </si>
   <si>
     <t>Total Frecuency</t>
+  </si>
+  <si>
+    <t>Search Terms &amp; Scope</t>
   </si>
 </sst>
 </file>
@@ -216,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -243,6 +240,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -343,11 +346,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="91163264"/>
-        <c:axId val="91169152"/>
+        <c:axId val="54356992"/>
+        <c:axId val="54358784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="91163264"/>
+        <c:axId val="54356992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -356,7 +359,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91169152"/>
+        <c:crossAx val="54358784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -364,7 +367,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91169152"/>
+        <c:axId val="54358784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -375,7 +378,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91163264"/>
+        <c:crossAx val="54356992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -622,11 +625,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="91181824"/>
-        <c:axId val="100813056"/>
+        <c:axId val="89899776"/>
+        <c:axId val="89901312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="91181824"/>
+        <c:axId val="89899776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -636,7 +639,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100813056"/>
+        <c:crossAx val="89901312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -644,7 +647,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100813056"/>
+        <c:axId val="89901312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -655,14 +658,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91181824"/>
+        <c:crossAx val="89899776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1079,7 +1081,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E3:M8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3:M3"/>
     </sheetView>
   </sheetViews>
@@ -1148,7 +1150,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -1177,7 +1179,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>2</v>
@@ -1196,7 +1198,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1204,32 +1206,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="29" style="18" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="8" t="s">
         <v>8</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1256,27 +1254,27 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>13</v>
-      </c>
       <c r="C1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>14</v>
-      </c>
       <c r="F1" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -1320,7 +1318,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1334,22 +1332,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>19</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>